<commit_message>
Remove company & country columns from spreadsheet
</commit_message>
<xml_diff>
--- a/resources/downloads/Argo Sales Tracker format.xlsx
+++ b/resources/downloads/Argo Sales Tracker format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evand\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evand\Desktop\Sales Tracker website\resources\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600D6D70-1B1A-404D-B1B1-C0BFAA28DBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57A8533-83E0-4874-BC93-63F0E9A35DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Purchases" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="62">
   <si>
     <t>Order #</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>Sale #</t>
-  </si>
-  <si>
-    <t>Country of destination</t>
   </si>
   <si>
     <t>Charged difference</t>
@@ -576,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -588,22 +585,20 @@
     <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.90625" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.1796875" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -617,256 +612,220 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="3">
+        <v>45703</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2">
+        <v>250</v>
+      </c>
+      <c r="H2" s="2">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2">
+        <v>20</v>
+      </c>
+      <c r="J2" s="2">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2">
+        <v>550</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="3">
-        <v>45703</v>
-      </c>
-      <c r="H2" s="2">
-        <v>2</v>
-      </c>
-      <c r="I2" s="2">
-        <v>250</v>
-      </c>
-      <c r="J2" s="2">
-        <v>25</v>
-      </c>
-      <c r="K2" s="2">
-        <v>20</v>
-      </c>
-      <c r="L2" s="2">
-        <v>5</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="2">
-        <v>0</v>
-      </c>
-      <c r="O2" s="2">
-        <v>550</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="3">
+        <v>40</v>
+      </c>
+      <c r="E3" s="3">
         <v>45703</v>
       </c>
-      <c r="H3" s="2">
+      <c r="F3" s="2">
         <v>4</v>
       </c>
-      <c r="I3" s="2">
+      <c r="G3" s="2">
         <v>150</v>
       </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="3">
+        <v>45703</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>800</v>
+      </c>
+      <c r="H4" s="2">
+        <v>45</v>
+      </c>
+      <c r="I4" s="2">
+        <v>72</v>
+      </c>
+      <c r="J4" s="2">
+        <v>10</v>
+      </c>
+      <c r="K4" s="2">
+        <v>50</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>2477</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="3">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="3">
         <v>45703</v>
       </c>
-      <c r="H4" s="2">
-        <v>3</v>
-      </c>
-      <c r="I4" s="2">
-        <v>800</v>
-      </c>
-      <c r="J4" s="2">
-        <v>45</v>
-      </c>
-      <c r="K4" s="2">
-        <v>72</v>
-      </c>
-      <c r="L4" s="2">
-        <v>10</v>
-      </c>
-      <c r="M4" s="2">
-        <v>50</v>
-      </c>
-      <c r="N4" s="2">
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>350</v>
+      </c>
+      <c r="H5" s="2">
+        <v>30</v>
+      </c>
+      <c r="I5" s="2">
+        <v>28</v>
+      </c>
+      <c r="J5" s="2">
         <v>0</v>
       </c>
-      <c r="O4" s="2">
-        <v>2477</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="3">
-        <v>45703</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2">
-        <v>350</v>
-      </c>
-      <c r="J5" s="2">
-        <v>30</v>
-      </c>
       <c r="K5" s="2">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="L5" s="2">
         <v>0</v>
       </c>
       <c r="M5" s="2">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0</v>
-      </c>
-      <c r="O5" s="2">
         <v>408</v>
       </c>
-      <c r="P5" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N5" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="C6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="E6" s="3">
         <v>45703</v>
       </c>
-      <c r="H6" s="2">
+      <c r="F6" s="2">
         <v>10</v>
       </c>
-      <c r="I6" s="2">
+      <c r="G6" s="2">
         <v>4.5</v>
       </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="G7" s="3"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -875,10 +834,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView zoomScale="89" workbookViewId="0">
+      <selection activeCell="F1" activeCellId="1" sqref="E1:E1048576 F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -887,21 +846,19 @@
     <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.26953125" customWidth="1"/>
-    <col min="16" max="16" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.1796875" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="3.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.26953125" customWidth="1"/>
+    <col min="14" max="14" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -915,253 +872,217 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="3">
+        <v>45703</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2">
+        <v>250</v>
+      </c>
+      <c r="H2" s="2">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2">
+        <v>20</v>
+      </c>
+      <c r="J2" s="2">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="3">
-        <v>45703</v>
-      </c>
-      <c r="H2" s="2">
-        <v>2</v>
-      </c>
-      <c r="I2" s="2">
-        <v>250</v>
-      </c>
-      <c r="J2" s="2">
-        <v>25</v>
-      </c>
       <c r="K2" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="L2" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M2" s="2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="2">
-        <v>0</v>
-      </c>
-      <c r="O2" s="2">
         <v>550</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N2" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="3">
+        <v>40</v>
+      </c>
+      <c r="E3" s="3">
         <v>45703</v>
       </c>
-      <c r="H3" s="2">
+      <c r="F3" s="2">
         <v>4</v>
       </c>
-      <c r="I3" s="2">
+      <c r="G3" s="2">
         <v>150</v>
       </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="3">
+        <v>45703</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>800</v>
+      </c>
+      <c r="H4" s="2">
+        <v>45</v>
+      </c>
+      <c r="I4" s="2">
+        <v>72</v>
+      </c>
+      <c r="J4" s="2">
+        <v>10</v>
+      </c>
+      <c r="K4" s="2">
+        <v>50</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>2477</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="3">
         <v>45703</v>
       </c>
-      <c r="H4" s="2">
-        <v>3</v>
-      </c>
-      <c r="I4" s="2">
-        <v>800</v>
-      </c>
-      <c r="J4" s="2">
-        <v>45</v>
-      </c>
-      <c r="K4" s="2">
-        <v>72</v>
-      </c>
-      <c r="L4" s="2">
-        <v>10</v>
-      </c>
-      <c r="M4" s="2">
-        <v>50</v>
-      </c>
-      <c r="N4" s="2">
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>350</v>
+      </c>
+      <c r="H5" s="2">
+        <v>30</v>
+      </c>
+      <c r="I5" s="2">
+        <v>28</v>
+      </c>
+      <c r="J5" s="2">
         <v>0</v>
       </c>
-      <c r="O4" s="2">
-        <v>2477</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="3">
-        <v>45703</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2">
-        <v>350</v>
-      </c>
-      <c r="J5" s="2">
-        <v>30</v>
-      </c>
       <c r="K5" s="2">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="L5" s="2">
         <v>0</v>
       </c>
       <c r="M5" s="2">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0</v>
-      </c>
-      <c r="O5" s="2">
         <v>408</v>
       </c>
-      <c r="P5" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N5" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="C6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="E6" s="3">
         <v>45703</v>
       </c>
-      <c r="H6" s="2">
+      <c r="F6" s="2">
         <v>10</v>
       </c>
-      <c r="I6" s="2">
+      <c r="G6" s="2">
         <v>4.5</v>
       </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1188,10 +1109,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -1205,87 +1126,87 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
         <v>42</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>43</v>
-      </c>
-      <c r="C4" t="s">
-        <v>44</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
         <v>49</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
         <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1312,10 +1233,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -1329,87 +1250,87 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
         <v>42</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>43</v>
-      </c>
-      <c r="C4" t="s">
-        <v>44</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
         <v>49</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
         <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1433,32 +1354,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1481,27 +1402,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>